<commit_message>
Starting of Monte-Carlo Development
</commit_message>
<xml_diff>
--- a/Code/trial2-pascascades-data.xlsx
+++ b/Code/trial2-pascascades-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="270">
   <si>
     <t>Drone #1_1</t>
   </si>
@@ -341,6 +341,411 @@
   </si>
   <si>
     <t>Drone #5_3</t>
+  </si>
+  <si>
+    <t>Drone #1</t>
+  </si>
+  <si>
+    <t>Drone #2</t>
+  </si>
+  <si>
+    <t>Drone #3</t>
+  </si>
+  <si>
+    <t>Drone #4</t>
+  </si>
+  <si>
+    <t>Drone #5</t>
+  </si>
+  <si>
+    <t>Drone #1</t>
+  </si>
+  <si>
+    <t>Drone #2</t>
+  </si>
+  <si>
+    <t>Drone #3</t>
+  </si>
+  <si>
+    <t>Drone #4</t>
+  </si>
+  <si>
+    <t>Drone #5</t>
+  </si>
+  <si>
+    <t>Fire #1</t>
+  </si>
+  <si>
+    <t>Fire #2</t>
+  </si>
+  <si>
+    <t>Fire #3</t>
+  </si>
+  <si>
+    <t>Fire #4</t>
+  </si>
+  <si>
+    <t>Fire #5</t>
+  </si>
+  <si>
+    <t>Fire #6</t>
+  </si>
+  <si>
+    <t>Fire #7</t>
+  </si>
+  <si>
+    <t>Fire #8</t>
+  </si>
+  <si>
+    <t>Fire #9</t>
+  </si>
+  <si>
+    <t>Fire #10</t>
+  </si>
+  <si>
+    <t>Fire #11</t>
+  </si>
+  <si>
+    <t>Fire #12</t>
+  </si>
+  <si>
+    <t>Fire #13</t>
+  </si>
+  <si>
+    <t>Fire #14</t>
+  </si>
+  <si>
+    <t>Fire #15</t>
+  </si>
+  <si>
+    <t>timeElapsed</t>
+  </si>
+  <si>
+    <t>Drone #1_1</t>
+  </si>
+  <si>
+    <t>Drone #1_2</t>
+  </si>
+  <si>
+    <t>Drone #1_3</t>
+  </si>
+  <si>
+    <t>Drone #1_4</t>
+  </si>
+  <si>
+    <t>Drone #2_1</t>
+  </si>
+  <si>
+    <t>Drone #2_2</t>
+  </si>
+  <si>
+    <t>Drone #2_3</t>
+  </si>
+  <si>
+    <t>Drone #2_4</t>
+  </si>
+  <si>
+    <t>Drone #2_5</t>
+  </si>
+  <si>
+    <t>Drone #3_1</t>
+  </si>
+  <si>
+    <t>Drone #3_2</t>
+  </si>
+  <si>
+    <t>Drone #3_3</t>
+  </si>
+  <si>
+    <t>Drone #3_4</t>
+  </si>
+  <si>
+    <t>Drone #3_5</t>
+  </si>
+  <si>
+    <t>Drone #3_6</t>
+  </si>
+  <si>
+    <t>Drone #3_7</t>
+  </si>
+  <si>
+    <t>Drone #4_1</t>
+  </si>
+  <si>
+    <t>Drone #4_2</t>
+  </si>
+  <si>
+    <t>Drone #5</t>
+  </si>
+  <si>
+    <t>Drone #1</t>
+  </si>
+  <si>
+    <t>Drone #2</t>
+  </si>
+  <si>
+    <t>Drone #3</t>
+  </si>
+  <si>
+    <t>Drone #4</t>
+  </si>
+  <si>
+    <t>Drone #5</t>
+  </si>
+  <si>
+    <t>Drone #1</t>
+  </si>
+  <si>
+    <t>Drone #2</t>
+  </si>
+  <si>
+    <t>Drone #3</t>
+  </si>
+  <si>
+    <t>Drone #4</t>
+  </si>
+  <si>
+    <t>Drone #5</t>
+  </si>
+  <si>
+    <t>Fire #1</t>
+  </si>
+  <si>
+    <t>Fire #2</t>
+  </si>
+  <si>
+    <t>Fire #3</t>
+  </si>
+  <si>
+    <t>Fire #4</t>
+  </si>
+  <si>
+    <t>Fire #5</t>
+  </si>
+  <si>
+    <t>Fire #6</t>
+  </si>
+  <si>
+    <t>Fire #7</t>
+  </si>
+  <si>
+    <t>Fire #8</t>
+  </si>
+  <si>
+    <t>Fire #9</t>
+  </si>
+  <si>
+    <t>Fire #10</t>
+  </si>
+  <si>
+    <t>Fire #11</t>
+  </si>
+  <si>
+    <t>Fire #12</t>
+  </si>
+  <si>
+    <t>Fire #13</t>
+  </si>
+  <si>
+    <t>Fire #14</t>
+  </si>
+  <si>
+    <t>Fire #15</t>
+  </si>
+  <si>
+    <t>timeElapsed</t>
+  </si>
+  <si>
+    <t>Drone #1_1</t>
+  </si>
+  <si>
+    <t>Drone #1_2</t>
+  </si>
+  <si>
+    <t>Drone #1_3</t>
+  </si>
+  <si>
+    <t>Drone #1_4</t>
+  </si>
+  <si>
+    <t>Drone #2_1</t>
+  </si>
+  <si>
+    <t>Drone #2_2</t>
+  </si>
+  <si>
+    <t>Drone #2_3</t>
+  </si>
+  <si>
+    <t>Drone #3_1</t>
+  </si>
+  <si>
+    <t>Drone #3_2</t>
+  </si>
+  <si>
+    <t>Drone #3_3</t>
+  </si>
+  <si>
+    <t>Drone #4_1</t>
+  </si>
+  <si>
+    <t>Drone #4_2</t>
+  </si>
+  <si>
+    <t>Drone #4_3</t>
+  </si>
+  <si>
+    <t>Drone #4_4</t>
+  </si>
+  <si>
+    <t>Drone #5_1</t>
+  </si>
+  <si>
+    <t>Drone #5_2</t>
+  </si>
+  <si>
+    <t>Drone #5_3</t>
+  </si>
+  <si>
+    <t>Drone #5_4</t>
+  </si>
+  <si>
+    <t>Drone #5_5</t>
+  </si>
+  <si>
+    <t>Drone #1</t>
+  </si>
+  <si>
+    <t>Drone #2</t>
+  </si>
+  <si>
+    <t>Drone #3</t>
+  </si>
+  <si>
+    <t>Drone #4</t>
+  </si>
+  <si>
+    <t>Drone #5</t>
+  </si>
+  <si>
+    <t>Drone #1</t>
+  </si>
+  <si>
+    <t>Drone #2</t>
+  </si>
+  <si>
+    <t>Drone #3</t>
+  </si>
+  <si>
+    <t>Drone #4</t>
+  </si>
+  <si>
+    <t>Drone #5</t>
+  </si>
+  <si>
+    <t>Fire #1</t>
+  </si>
+  <si>
+    <t>Fire #2</t>
+  </si>
+  <si>
+    <t>Fire #3</t>
+  </si>
+  <si>
+    <t>Fire #4</t>
+  </si>
+  <si>
+    <t>Fire #5</t>
+  </si>
+  <si>
+    <t>Fire #6</t>
+  </si>
+  <si>
+    <t>Fire #7</t>
+  </si>
+  <si>
+    <t>Fire #8</t>
+  </si>
+  <si>
+    <t>Fire #9</t>
+  </si>
+  <si>
+    <t>Fire #10</t>
+  </si>
+  <si>
+    <t>Fire #11</t>
+  </si>
+  <si>
+    <t>Fire #12</t>
+  </si>
+  <si>
+    <t>Fire #13</t>
+  </si>
+  <si>
+    <t>Fire #14</t>
+  </si>
+  <si>
+    <t>Fire #15</t>
+  </si>
+  <si>
+    <t>timeElapsed</t>
+  </si>
+  <si>
+    <t>Drone #1_1</t>
+  </si>
+  <si>
+    <t>Drone #1_2</t>
+  </si>
+  <si>
+    <t>Drone #1_3</t>
+  </si>
+  <si>
+    <t>Drone #2_1</t>
+  </si>
+  <si>
+    <t>Drone #2_2</t>
+  </si>
+  <si>
+    <t>Drone #2_3</t>
+  </si>
+  <si>
+    <t>Drone #2_4</t>
+  </si>
+  <si>
+    <t>Drone #2_5</t>
+  </si>
+  <si>
+    <t>Drone #3_1</t>
+  </si>
+  <si>
+    <t>Drone #3_2</t>
+  </si>
+  <si>
+    <t>Drone #3_3</t>
+  </si>
+  <si>
+    <t>Drone #3_4</t>
+  </si>
+  <si>
+    <t>Drone #3_5</t>
+  </si>
+  <si>
+    <t>Drone #3_6</t>
+  </si>
+  <si>
+    <t>Drone #4_1</t>
+  </si>
+  <si>
+    <t>Drone #4_2</t>
+  </si>
+  <si>
+    <t>Drone #4_3</t>
+  </si>
+  <si>
+    <t>Drone #4_4</t>
+  </si>
+  <si>
+    <t>Drone #5</t>
   </si>
   <si>
     <t>Drone #1</t>
@@ -439,7 +844,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -462,11 +867,26 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -483,6 +903,21 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,66 +948,66 @@
     <col min="16" max="16" width="10.34375" customWidth="true"/>
     <col min="17" max="17" width="10.34375" customWidth="true"/>
     <col min="18" max="18" width="10.34375" customWidth="true"/>
-    <col min="19" max="19" width="10.34375" customWidth="true"/>
+    <col min="19" max="19" width="8.3984375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>91</v>
+        <v>226</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>92</v>
+        <v>227</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>93</v>
+        <v>228</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>94</v>
+        <v>229</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>95</v>
+        <v>230</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>96</v>
+        <v>231</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>97</v>
+        <v>232</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>98</v>
+        <v>233</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>99</v>
+        <v>234</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>100</v>
+        <v>235</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>101</v>
+        <v>236</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>102</v>
+        <v>237</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>103</v>
+        <v>238</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>104</v>
+        <v>239</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>105</v>
+        <v>240</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>106</v>
+        <v>241</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>107</v>
+        <v>242</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>108</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2">
@@ -589,66 +1024,66 @@
         <v>3</v>
       </c>
       <c r="E2" s="0">
+        <v>12</v>
+      </c>
+      <c r="F2" s="0">
         <v>4</v>
       </c>
-      <c r="F2" s="0">
+      <c r="G2" s="0">
         <v>13</v>
-      </c>
-      <c r="G2" s="0">
-        <v>12</v>
       </c>
       <c r="H2" s="0">
         <v>1.0165236051502147</v>
       </c>
       <c r="I2" s="0">
+        <v>10</v>
+      </c>
+      <c r="J2" s="0">
+        <v>9</v>
+      </c>
+      <c r="K2" s="0">
         <v>11</v>
       </c>
-      <c r="J2" s="0">
-        <v>10</v>
-      </c>
-      <c r="K2" s="0">
+      <c r="L2" s="0">
         <v>5</v>
-      </c>
-      <c r="L2" s="0">
-        <v>1.2783261802575105</v>
       </c>
       <c r="M2" s="0">
         <v>14</v>
       </c>
       <c r="N2" s="0">
+        <v>1.1763948497854075</v>
+      </c>
+      <c r="O2" s="0">
+        <v>6</v>
+      </c>
+      <c r="P2" s="0">
         <v>8</v>
       </c>
-      <c r="O2" s="0">
-        <v>9</v>
-      </c>
-      <c r="P2" s="0">
-        <v>1.3158798283261801</v>
-      </c>
       <c r="Q2" s="0">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="R2" s="0">
-        <v>1.3877682403433478</v>
+        <v>1.3620171673819743</v>
       </c>
       <c r="S2" s="0">
-        <v>15.999999999999988</v>
+        <v>1.4435622317596568</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>109</v>
+        <v>244</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>110</v>
+        <v>245</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>111</v>
+        <v>246</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>112</v>
+        <v>247</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>113</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5">
@@ -670,19 +1105,19 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>114</v>
+        <v>249</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>115</v>
+        <v>250</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>116</v>
+        <v>251</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>117</v>
+        <v>252</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>118</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8">
@@ -690,63 +1125,63 @@
         <v>5.0300457761935355</v>
       </c>
       <c r="B8" s="0">
-        <v>7.6905854175592605</v>
+        <v>7.6905854175592614</v>
       </c>
       <c r="C8" s="0">
-        <v>17.86482874670164</v>
+        <v>18.088222917612036</v>
       </c>
       <c r="D8" s="0">
-        <v>19.80687208738804</v>
+        <v>22.214266349095453</v>
       </c>
       <c r="E8" s="0">
-        <v>22.615119834714157</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>119</v>
+        <v>254</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>120</v>
+        <v>255</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>121</v>
+        <v>256</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>122</v>
+        <v>257</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>123</v>
+        <v>258</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>124</v>
+        <v>259</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>125</v>
+        <v>260</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>126</v>
+        <v>261</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>127</v>
+        <v>262</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>128</v>
+        <v>263</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>129</v>
+        <v>264</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>130</v>
+        <v>265</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>131</v>
+        <v>266</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>132</v>
+        <v>267</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>133</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11">
@@ -798,12 +1233,12 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>134</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>27.3685464</v>
+        <v>23.3089218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing with pheromone parameter
</commit_message>
<xml_diff>
--- a/Code/trial2-pascascades-data.xlsx
+++ b/Code/trial2-pascascades-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="385">
   <si>
     <t>Drone #1_1</t>
   </si>
@@ -821,6 +821,351 @@
   </si>
   <si>
     <t>Fire #15</t>
+  </si>
+  <si>
+    <t>timeElapsed</t>
+  </si>
+  <si>
+    <t>Drone #1_1</t>
+  </si>
+  <si>
+    <t>Drone #1_2</t>
+  </si>
+  <si>
+    <t>Drone #1_3</t>
+  </si>
+  <si>
+    <t>Drone #1_4</t>
+  </si>
+  <si>
+    <t>Drone #1_5</t>
+  </si>
+  <si>
+    <t>Drone #2_1</t>
+  </si>
+  <si>
+    <t>Drone #2_2</t>
+  </si>
+  <si>
+    <t>Drone #2_3</t>
+  </si>
+  <si>
+    <t>Drone #2_4</t>
+  </si>
+  <si>
+    <t>Drone #2_5</t>
+  </si>
+  <si>
+    <t>Drone #2_6</t>
+  </si>
+  <si>
+    <t>Drone #2_7</t>
+  </si>
+  <si>
+    <t>Drone #2_8</t>
+  </si>
+  <si>
+    <t>Drone #2_9</t>
+  </si>
+  <si>
+    <t>Drone #3_1</t>
+  </si>
+  <si>
+    <t>Drone #3_2</t>
+  </si>
+  <si>
+    <t>Drone #3_3</t>
+  </si>
+  <si>
+    <t>Drone #3_4</t>
+  </si>
+  <si>
+    <t>Drone #3_5</t>
+  </si>
+  <si>
+    <t>Drone #3_6</t>
+  </si>
+  <si>
+    <t>Drone #3_7</t>
+  </si>
+  <si>
+    <t>Drone #4_ 1</t>
+  </si>
+  <si>
+    <t>Drone #4_ 2</t>
+  </si>
+  <si>
+    <t>Drone #4_ 3</t>
+  </si>
+  <si>
+    <t>Drone #4_ 4</t>
+  </si>
+  <si>
+    <t>Drone #4_ 5</t>
+  </si>
+  <si>
+    <t>Drone #4_ 6</t>
+  </si>
+  <si>
+    <t>Drone #4_ 7</t>
+  </si>
+  <si>
+    <t>Drone #4_ 8</t>
+  </si>
+  <si>
+    <t>Drone #4_ 9</t>
+  </si>
+  <si>
+    <t>Drone #4_10</t>
+  </si>
+  <si>
+    <t>Drone #4_11</t>
+  </si>
+  <si>
+    <t>Drone #4_12</t>
+  </si>
+  <si>
+    <t>Drone #4_13</t>
+  </si>
+  <si>
+    <t>Drone #5_ 1</t>
+  </si>
+  <si>
+    <t>Drone #5_ 2</t>
+  </si>
+  <si>
+    <t>Drone #5_ 3</t>
+  </si>
+  <si>
+    <t>Drone #5_ 4</t>
+  </si>
+  <si>
+    <t>Drone #5_ 5</t>
+  </si>
+  <si>
+    <t>Drone #5_ 6</t>
+  </si>
+  <si>
+    <t>Drone #5_ 7</t>
+  </si>
+  <si>
+    <t>Drone #5_ 8</t>
+  </si>
+  <si>
+    <t>Drone #5_ 9</t>
+  </si>
+  <si>
+    <t>Drone #5_10</t>
+  </si>
+  <si>
+    <t>Drone #5_11</t>
+  </si>
+  <si>
+    <t>Drone #5_12</t>
+  </si>
+  <si>
+    <t>Drone #5_13</t>
+  </si>
+  <si>
+    <t>Drone #5_14</t>
+  </si>
+  <si>
+    <t>Drone #5_15</t>
+  </si>
+  <si>
+    <t>Drone #5_16</t>
+  </si>
+  <si>
+    <t>Drone #5_17</t>
+  </si>
+  <si>
+    <t>Drone #5_18</t>
+  </si>
+  <si>
+    <t>Drone #5_19</t>
+  </si>
+  <si>
+    <t>Drone #5_20</t>
+  </si>
+  <si>
+    <t>Drone #1</t>
+  </si>
+  <si>
+    <t>Drone #2</t>
+  </si>
+  <si>
+    <t>Drone #3</t>
+  </si>
+  <si>
+    <t>Drone #4</t>
+  </si>
+  <si>
+    <t>Drone #5</t>
+  </si>
+  <si>
+    <t>Drone #1</t>
+  </si>
+  <si>
+    <t>Drone #2</t>
+  </si>
+  <si>
+    <t>Drone #3</t>
+  </si>
+  <si>
+    <t>Drone #4</t>
+  </si>
+  <si>
+    <t>Drone #5</t>
+  </si>
+  <si>
+    <t>Fire #1</t>
+  </si>
+  <si>
+    <t>Fire #2</t>
+  </si>
+  <si>
+    <t>Fire #3</t>
+  </si>
+  <si>
+    <t>Fire #4</t>
+  </si>
+  <si>
+    <t>Fire #5</t>
+  </si>
+  <si>
+    <t>Fire #6</t>
+  </si>
+  <si>
+    <t>Fire #7</t>
+  </si>
+  <si>
+    <t>Fire #8</t>
+  </si>
+  <si>
+    <t>Fire #9</t>
+  </si>
+  <si>
+    <t>Fire #10</t>
+  </si>
+  <si>
+    <t>Fire #11</t>
+  </si>
+  <si>
+    <t>Fire #12</t>
+  </si>
+  <si>
+    <t>Fire #13</t>
+  </si>
+  <si>
+    <t>Fire #14</t>
+  </si>
+  <si>
+    <t>Fire #15</t>
+  </si>
+  <si>
+    <t>Fire #16</t>
+  </si>
+  <si>
+    <t>Fire #17</t>
+  </si>
+  <si>
+    <t>Fire #18</t>
+  </si>
+  <si>
+    <t>Fire #19</t>
+  </si>
+  <si>
+    <t>Fire #20</t>
+  </si>
+  <si>
+    <t>Fire #21</t>
+  </si>
+  <si>
+    <t>Fire #22</t>
+  </si>
+  <si>
+    <t>Fire #23</t>
+  </si>
+  <si>
+    <t>Fire #24</t>
+  </si>
+  <si>
+    <t>Fire #25</t>
+  </si>
+  <si>
+    <t>Fire #26</t>
+  </si>
+  <si>
+    <t>Fire #27</t>
+  </si>
+  <si>
+    <t>Fire #28</t>
+  </si>
+  <si>
+    <t>Fire #29</t>
+  </si>
+  <si>
+    <t>Fire #30</t>
+  </si>
+  <si>
+    <t>Fire #31</t>
+  </si>
+  <si>
+    <t>Fire #32</t>
+  </si>
+  <si>
+    <t>Fire #33</t>
+  </si>
+  <si>
+    <t>Fire #34</t>
+  </si>
+  <si>
+    <t>Fire #35</t>
+  </si>
+  <si>
+    <t>Fire #36</t>
+  </si>
+  <si>
+    <t>Fire #37</t>
+  </si>
+  <si>
+    <t>Fire #38</t>
+  </si>
+  <si>
+    <t>Fire #39</t>
+  </si>
+  <si>
+    <t>Fire #40</t>
+  </si>
+  <si>
+    <t>Fire #41</t>
+  </si>
+  <si>
+    <t>Fire #42</t>
+  </si>
+  <si>
+    <t>Fire #43</t>
+  </si>
+  <si>
+    <t>Fire #44</t>
+  </si>
+  <si>
+    <t>Fire #45</t>
+  </si>
+  <si>
+    <t>Fire #46</t>
+  </si>
+  <si>
+    <t>Fire #47</t>
+  </si>
+  <si>
+    <t>Fire #48</t>
+  </si>
+  <si>
+    <t>Fire #49</t>
+  </si>
+  <si>
+    <t>Fire #50</t>
   </si>
   <si>
     <t>timeElapsed</t>
@@ -844,7 +1189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -882,11 +1227,16 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -918,6 +1268,11 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,7 +1282,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:BB14"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="true"/>
@@ -945,300 +1300,755 @@
     <col min="13" max="13" width="7.44921875" customWidth="true"/>
     <col min="14" max="14" width="7.44921875" customWidth="true"/>
     <col min="15" max="15" width="7.44921875" customWidth="true"/>
-    <col min="16" max="16" width="10.34375" customWidth="true"/>
-    <col min="17" max="17" width="10.34375" customWidth="true"/>
-    <col min="18" max="18" width="10.34375" customWidth="true"/>
-    <col min="19" max="19" width="8.3984375" customWidth="true"/>
+    <col min="16" max="16" width="7.44921875" customWidth="true"/>
+    <col min="17" max="17" width="7.44921875" customWidth="true"/>
+    <col min="18" max="18" width="7.44921875" customWidth="true"/>
+    <col min="19" max="19" width="7.44921875" customWidth="true"/>
+    <col min="20" max="20" width="7.44921875" customWidth="true"/>
+    <col min="21" max="21" width="7.44921875" customWidth="true"/>
+    <col min="22" max="22" width="7.44921875" customWidth="true"/>
+    <col min="23" max="23" width="7.44921875" customWidth="true"/>
+    <col min="24" max="24" width="7.44921875" customWidth="true"/>
+    <col min="25" max="25" width="7.44921875" customWidth="true"/>
+    <col min="26" max="26" width="7.44921875" customWidth="true"/>
+    <col min="27" max="27" width="7.44921875" customWidth="true"/>
+    <col min="28" max="28" width="7.44921875" customWidth="true"/>
+    <col min="29" max="29" width="7.44921875" customWidth="true"/>
+    <col min="30" max="30" width="7.44921875" customWidth="true"/>
+    <col min="31" max="31" width="7.44921875" customWidth="true"/>
+    <col min="32" max="32" width="7.44921875" customWidth="true"/>
+    <col min="33" max="33" width="7.44921875" customWidth="true"/>
+    <col min="34" max="34" width="7.44921875" customWidth="true"/>
+    <col min="35" max="35" width="7.44921875" customWidth="true"/>
+    <col min="36" max="36" width="7.44921875" customWidth="true"/>
+    <col min="37" max="37" width="7.44921875" customWidth="true"/>
+    <col min="38" max="38" width="7.44921875" customWidth="true"/>
+    <col min="39" max="39" width="7.44921875" customWidth="true"/>
+    <col min="40" max="40" width="7.44921875" customWidth="true"/>
+    <col min="41" max="41" width="7.44921875" customWidth="true"/>
+    <col min="42" max="42" width="7.44921875" customWidth="true"/>
+    <col min="43" max="43" width="7.44921875" customWidth="true"/>
+    <col min="44" max="44" width="7.44921875" customWidth="true"/>
+    <col min="45" max="45" width="7.44921875" customWidth="true"/>
+    <col min="46" max="46" width="7.44921875" customWidth="true"/>
+    <col min="47" max="47" width="7.44921875" customWidth="true"/>
+    <col min="48" max="48" width="7.44921875" customWidth="true"/>
+    <col min="49" max="49" width="7.44921875" customWidth="true"/>
+    <col min="50" max="50" width="7.44921875" customWidth="true"/>
+    <col min="51" max="51" width="11.34375" customWidth="true"/>
+    <col min="52" max="52" width="11.34375" customWidth="true"/>
+    <col min="53" max="53" width="11.34375" customWidth="true"/>
+    <col min="54" max="54" width="11.34375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>226</v>
+        <v>271</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>227</v>
+        <v>272</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>229</v>
+        <v>274</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>230</v>
+        <v>275</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>231</v>
+        <v>276</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>232</v>
+        <v>277</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>233</v>
+        <v>278</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>234</v>
+        <v>279</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>235</v>
+        <v>280</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>236</v>
+        <v>281</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>237</v>
+        <v>282</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>238</v>
+        <v>283</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>239</v>
+        <v>284</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>240</v>
+        <v>285</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>241</v>
+        <v>286</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>242</v>
+        <v>287</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>243</v>
+        <v>288</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="AG1" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="AH1" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="AI1" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="AK1" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="AL1" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="AM1" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="AN1" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="AO1" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="AP1" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="AQ1" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="AR1" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="AS1" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="AT1" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="AU1" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="AV1" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="AW1" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="AX1" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="AY1" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="AZ1" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="BA1" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="BB1" s="0" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B2" s="0">
         <v>7</v>
       </c>
       <c r="C2" s="0">
-        <v>1.0015021459227467</v>
+        <v>27</v>
       </c>
       <c r="D2" s="0">
+        <v>44</v>
+      </c>
+      <c r="E2" s="0">
+        <v>14.424203821656048</v>
+      </c>
+      <c r="F2" s="0">
+        <v>19</v>
+      </c>
+      <c r="G2" s="0">
+        <v>16</v>
+      </c>
+      <c r="H2" s="0">
+        <v>17</v>
+      </c>
+      <c r="I2" s="0">
         <v>3</v>
       </c>
-      <c r="E2" s="0">
+      <c r="J2" s="0">
+        <v>28</v>
+      </c>
+      <c r="K2" s="0">
+        <v>34</v>
+      </c>
+      <c r="L2" s="0">
+        <v>32</v>
+      </c>
+      <c r="M2" s="0">
+        <v>14.575796178343952</v>
+      </c>
+      <c r="N2" s="0">
+        <v>26.041818181818179</v>
+      </c>
+      <c r="O2" s="0">
+        <v>40</v>
+      </c>
+      <c r="P2" s="0">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="0">
+        <v>22</v>
+      </c>
+      <c r="R2" s="0">
+        <v>1</v>
+      </c>
+      <c r="S2" s="0">
+        <v>18</v>
+      </c>
+      <c r="T2" s="0">
+        <v>36</v>
+      </c>
+      <c r="U2" s="0">
+        <v>26.120909090909095</v>
+      </c>
+      <c r="V2" s="0">
+        <v>49</v>
+      </c>
+      <c r="W2" s="0">
+        <v>39</v>
+      </c>
+      <c r="X2" s="0">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="0">
+        <v>11</v>
+      </c>
+      <c r="Z2" s="0">
+        <v>47</v>
+      </c>
+      <c r="AA2" s="0">
+        <v>21</v>
+      </c>
+      <c r="AB2" s="0">
+        <v>20</v>
+      </c>
+      <c r="AC2" s="0">
+        <v>33</v>
+      </c>
+      <c r="AD2" s="0">
+        <v>50</v>
+      </c>
+      <c r="AE2" s="0">
+        <v>24</v>
+      </c>
+      <c r="AF2" s="0">
+        <v>26.83727272727273</v>
+      </c>
+      <c r="AG2" s="0">
+        <v>29</v>
+      </c>
+      <c r="AH2" s="0">
+        <v>41.882666666666665</v>
+      </c>
+      <c r="AI2" s="0">
+        <v>9</v>
+      </c>
+      <c r="AJ2" s="0">
         <v>12</v>
       </c>
-      <c r="F2" s="0">
+      <c r="AK2" s="0">
+        <v>43</v>
+      </c>
+      <c r="AL2" s="0">
+        <v>37</v>
+      </c>
+      <c r="AM2" s="0">
+        <v>15</v>
+      </c>
+      <c r="AN2" s="0">
+        <v>25</v>
+      </c>
+      <c r="AO2" s="0">
+        <v>5</v>
+      </c>
+      <c r="AP2" s="0">
+        <v>2</v>
+      </c>
+      <c r="AQ2" s="0">
+        <v>48</v>
+      </c>
+      <c r="AR2" s="0">
+        <v>13</v>
+      </c>
+      <c r="AS2" s="0">
+        <v>31</v>
+      </c>
+      <c r="AT2" s="0">
+        <v>8</v>
+      </c>
+      <c r="AU2" s="0">
         <v>4</v>
       </c>
-      <c r="G2" s="0">
-        <v>13</v>
-      </c>
-      <c r="H2" s="0">
-        <v>1.0165236051502147</v>
-      </c>
-      <c r="I2" s="0">
-        <v>10</v>
-      </c>
-      <c r="J2" s="0">
-        <v>9</v>
-      </c>
-      <c r="K2" s="0">
-        <v>11</v>
-      </c>
-      <c r="L2" s="0">
-        <v>5</v>
-      </c>
-      <c r="M2" s="0">
-        <v>14</v>
-      </c>
-      <c r="N2" s="0">
-        <v>1.1763948497854075</v>
-      </c>
-      <c r="O2" s="0">
+      <c r="AV2" s="0">
+        <v>46</v>
+      </c>
+      <c r="AW2" s="0">
+        <v>35</v>
+      </c>
+      <c r="AX2" s="0">
+        <v>30</v>
+      </c>
+      <c r="AY2" s="0">
         <v>6</v>
       </c>
-      <c r="P2" s="0">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="0">
-        <v>15</v>
-      </c>
-      <c r="R2" s="0">
-        <v>1.3620171673819743</v>
-      </c>
-      <c r="S2" s="0">
-        <v>1.4435622317596568</v>
+      <c r="AZ2" s="0">
+        <v>45</v>
+      </c>
+      <c r="BA2" s="0">
+        <v>41.117333333333335</v>
+      </c>
+      <c r="BB2" s="0">
+        <v>42.999999999999993</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>244</v>
+        <v>324</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>245</v>
+        <v>325</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>246</v>
+        <v>326</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>247</v>
+        <v>327</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>248</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>20.669999999999998</v>
+        <v>63.665999999999997</v>
       </c>
       <c r="B5" s="0">
-        <v>20.669999999999998</v>
+        <v>63.665999999999997</v>
       </c>
       <c r="C5" s="0">
-        <v>20.669999999999998</v>
+        <v>63.665999999999997</v>
       </c>
       <c r="D5" s="0">
-        <v>20.669999999999998</v>
+        <v>63.665999999999997</v>
       </c>
       <c r="E5" s="0">
-        <v>20.669999999999998</v>
+        <v>63.665999999999997</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>249</v>
+        <v>329</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>250</v>
+        <v>330</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>251</v>
+        <v>331</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>252</v>
+        <v>332</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>253</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>5.0300457761935355</v>
+        <v>12.384320673308093</v>
       </c>
       <c r="B8" s="0">
-        <v>7.6905854175592614</v>
+        <v>14.074360601299274</v>
       </c>
       <c r="C8" s="0">
-        <v>18.088222917612036</v>
+        <v>13.134830942076498</v>
       </c>
       <c r="D8" s="0">
-        <v>22.214266349095453</v>
+        <v>20.237962497613381</v>
       </c>
       <c r="E8" s="0">
-        <v>10000</v>
+        <v>33.702802358954727</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>254</v>
+        <v>334</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>255</v>
+        <v>335</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>256</v>
+        <v>336</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>257</v>
+        <v>337</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>258</v>
+        <v>338</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>259</v>
+        <v>339</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>260</v>
+        <v>340</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>261</v>
+        <v>341</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>262</v>
+        <v>342</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>263</v>
+        <v>343</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>264</v>
+        <v>344</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>265</v>
+        <v>345</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>266</v>
+        <v>346</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>267</v>
+        <v>347</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>268</v>
+        <v>348</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="W10" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="Y10" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="Z10" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="AA10" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="AB10" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="AC10" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="AD10" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="AE10" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="AF10" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="AG10" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="AH10" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="AI10" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="AJ10" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="AK10" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="AL10" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="AM10" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="AN10" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="AO10" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="AP10" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="AQ10" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="AR10" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="AS10" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="AT10" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="AU10" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="AV10" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="AW10" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="AX10" s="0" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>46.600000000000001</v>
+        <v>24.600000000000001</v>
       </c>
       <c r="B11" s="0">
+        <v>1.3</v>
+      </c>
+      <c r="C11" s="0">
+        <v>7</v>
+      </c>
+      <c r="D11" s="0">
+        <v>5.7000000000000002</v>
+      </c>
+      <c r="E11" s="0">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F11" s="0">
+        <v>7</v>
+      </c>
+      <c r="G11" s="0">
+        <v>5</v>
+      </c>
+      <c r="H11" s="0">
+        <v>1.8</v>
+      </c>
+      <c r="I11" s="0">
+        <v>2</v>
+      </c>
+      <c r="J11" s="0">
+        <v>7.5999999999999996</v>
+      </c>
+      <c r="K11" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="L11" s="0">
+        <v>2</v>
+      </c>
+      <c r="M11" s="0">
+        <v>12</v>
+      </c>
+      <c r="N11" s="0">
+        <v>1.5700000000000001</v>
+      </c>
+      <c r="O11" s="0">
+        <v>5</v>
+      </c>
+      <c r="P11" s="0">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="Q11" s="0">
+        <v>8.5</v>
+      </c>
+      <c r="R11" s="0">
+        <v>8.5</v>
+      </c>
+      <c r="S11" s="0">
+        <v>5</v>
+      </c>
+      <c r="T11" s="0">
+        <v>14</v>
+      </c>
+      <c r="U11" s="0">
+        <v>1</v>
+      </c>
+      <c r="V11" s="0">
+        <v>16.699999999999999</v>
+      </c>
+      <c r="W11" s="0">
+        <v>33</v>
+      </c>
+      <c r="X11" s="0">
+        <v>11</v>
+      </c>
+      <c r="Y11" s="0">
+        <v>1.3</v>
+      </c>
+      <c r="Z11" s="0">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AA11" s="0">
+        <v>21</v>
+      </c>
+      <c r="AB11" s="0">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="AC11" s="0">
+        <v>1.2</v>
+      </c>
+      <c r="AD11" s="0">
+        <v>2</v>
+      </c>
+      <c r="AE11" s="0">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AG11" s="0">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AH11" s="0">
+        <v>1.27</v>
+      </c>
+      <c r="AI11" s="0">
+        <v>2.7999999999999998</v>
+      </c>
+      <c r="AJ11" s="0">
+        <v>5</v>
+      </c>
+      <c r="AK11" s="0">
         <v>2.1000000000000001</v>
       </c>
-      <c r="C11" s="0">
+      <c r="AL11" s="0">
+        <v>10.4</v>
+      </c>
+      <c r="AM11" s="0">
+        <v>3</v>
+      </c>
+      <c r="AN11" s="0">
+        <v>1</v>
+      </c>
+      <c r="AO11" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="AP11" s="0">
+        <v>2</v>
+      </c>
+      <c r="AQ11" s="0">
+        <v>3.3900000000000001</v>
+      </c>
+      <c r="AR11" s="0">
         <v>4</v>
       </c>
-      <c r="D11" s="0">
-        <v>9.9000000000000004</v>
-      </c>
-      <c r="E11" s="0">
-        <v>2.8999999999999999</v>
-      </c>
-      <c r="F11" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G11" s="0">
-        <v>18.5</v>
-      </c>
-      <c r="H11" s="0">
-        <v>1.2</v>
-      </c>
-      <c r="I11" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="J11" s="0">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="K11" s="0">
+      <c r="AS11" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="AT11" s="0">
+        <v>2</v>
+      </c>
+      <c r="AU11" s="0">
+        <v>1.7</v>
+      </c>
+      <c r="AV11" s="0">
+        <v>5.4000000000000004</v>
+      </c>
+      <c r="AW11" s="0">
+        <v>9</v>
+      </c>
+      <c r="AX11" s="0">
         <v>2.6000000000000001</v>
-      </c>
-      <c r="L11" s="0">
-        <v>1</v>
-      </c>
-      <c r="M11" s="0">
-        <v>5</v>
-      </c>
-      <c r="N11" s="0">
-        <v>3.25</v>
-      </c>
-      <c r="O11" s="0">
-        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>269</v>
+        <v>384</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>23.3089218</v>
+        <v>104.1449846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of a greedy baseline
</commit_message>
<xml_diff>
--- a/Code/trial2-pascascades-data.xlsx
+++ b/Code/trial2-pascascades-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="500">
   <si>
     <t>Drone #1_1</t>
   </si>
@@ -821,6 +821,351 @@
   </si>
   <si>
     <t>Fire #15</t>
+  </si>
+  <si>
+    <t>timeElapsed</t>
+  </si>
+  <si>
+    <t>Drone #1_1</t>
+  </si>
+  <si>
+    <t>Drone #1_2</t>
+  </si>
+  <si>
+    <t>Drone #1_3</t>
+  </si>
+  <si>
+    <t>Drone #1_4</t>
+  </si>
+  <si>
+    <t>Drone #1_5</t>
+  </si>
+  <si>
+    <t>Drone #2_1</t>
+  </si>
+  <si>
+    <t>Drone #2_2</t>
+  </si>
+  <si>
+    <t>Drone #2_3</t>
+  </si>
+  <si>
+    <t>Drone #2_4</t>
+  </si>
+  <si>
+    <t>Drone #2_5</t>
+  </si>
+  <si>
+    <t>Drone #2_6</t>
+  </si>
+  <si>
+    <t>Drone #2_7</t>
+  </si>
+  <si>
+    <t>Drone #2_8</t>
+  </si>
+  <si>
+    <t>Drone #2_9</t>
+  </si>
+  <si>
+    <t>Drone #3_1</t>
+  </si>
+  <si>
+    <t>Drone #3_2</t>
+  </si>
+  <si>
+    <t>Drone #3_3</t>
+  </si>
+  <si>
+    <t>Drone #3_4</t>
+  </si>
+  <si>
+    <t>Drone #3_5</t>
+  </si>
+  <si>
+    <t>Drone #3_6</t>
+  </si>
+  <si>
+    <t>Drone #3_7</t>
+  </si>
+  <si>
+    <t>Drone #4_ 1</t>
+  </si>
+  <si>
+    <t>Drone #4_ 2</t>
+  </si>
+  <si>
+    <t>Drone #4_ 3</t>
+  </si>
+  <si>
+    <t>Drone #4_ 4</t>
+  </si>
+  <si>
+    <t>Drone #4_ 5</t>
+  </si>
+  <si>
+    <t>Drone #4_ 6</t>
+  </si>
+  <si>
+    <t>Drone #4_ 7</t>
+  </si>
+  <si>
+    <t>Drone #4_ 8</t>
+  </si>
+  <si>
+    <t>Drone #4_ 9</t>
+  </si>
+  <si>
+    <t>Drone #4_10</t>
+  </si>
+  <si>
+    <t>Drone #4_11</t>
+  </si>
+  <si>
+    <t>Drone #4_12</t>
+  </si>
+  <si>
+    <t>Drone #4_13</t>
+  </si>
+  <si>
+    <t>Drone #5_ 1</t>
+  </si>
+  <si>
+    <t>Drone #5_ 2</t>
+  </si>
+  <si>
+    <t>Drone #5_ 3</t>
+  </si>
+  <si>
+    <t>Drone #5_ 4</t>
+  </si>
+  <si>
+    <t>Drone #5_ 5</t>
+  </si>
+  <si>
+    <t>Drone #5_ 6</t>
+  </si>
+  <si>
+    <t>Drone #5_ 7</t>
+  </si>
+  <si>
+    <t>Drone #5_ 8</t>
+  </si>
+  <si>
+    <t>Drone #5_ 9</t>
+  </si>
+  <si>
+    <t>Drone #5_10</t>
+  </si>
+  <si>
+    <t>Drone #5_11</t>
+  </si>
+  <si>
+    <t>Drone #5_12</t>
+  </si>
+  <si>
+    <t>Drone #5_13</t>
+  </si>
+  <si>
+    <t>Drone #5_14</t>
+  </si>
+  <si>
+    <t>Drone #5_15</t>
+  </si>
+  <si>
+    <t>Drone #5_16</t>
+  </si>
+  <si>
+    <t>Drone #5_17</t>
+  </si>
+  <si>
+    <t>Drone #5_18</t>
+  </si>
+  <si>
+    <t>Drone #5_19</t>
+  </si>
+  <si>
+    <t>Drone #5_20</t>
+  </si>
+  <si>
+    <t>Drone #1</t>
+  </si>
+  <si>
+    <t>Drone #2</t>
+  </si>
+  <si>
+    <t>Drone #3</t>
+  </si>
+  <si>
+    <t>Drone #4</t>
+  </si>
+  <si>
+    <t>Drone #5</t>
+  </si>
+  <si>
+    <t>Drone #1</t>
+  </si>
+  <si>
+    <t>Drone #2</t>
+  </si>
+  <si>
+    <t>Drone #3</t>
+  </si>
+  <si>
+    <t>Drone #4</t>
+  </si>
+  <si>
+    <t>Drone #5</t>
+  </si>
+  <si>
+    <t>Fire #1</t>
+  </si>
+  <si>
+    <t>Fire #2</t>
+  </si>
+  <si>
+    <t>Fire #3</t>
+  </si>
+  <si>
+    <t>Fire #4</t>
+  </si>
+  <si>
+    <t>Fire #5</t>
+  </si>
+  <si>
+    <t>Fire #6</t>
+  </si>
+  <si>
+    <t>Fire #7</t>
+  </si>
+  <si>
+    <t>Fire #8</t>
+  </si>
+  <si>
+    <t>Fire #9</t>
+  </si>
+  <si>
+    <t>Fire #10</t>
+  </si>
+  <si>
+    <t>Fire #11</t>
+  </si>
+  <si>
+    <t>Fire #12</t>
+  </si>
+  <si>
+    <t>Fire #13</t>
+  </si>
+  <si>
+    <t>Fire #14</t>
+  </si>
+  <si>
+    <t>Fire #15</t>
+  </si>
+  <si>
+    <t>Fire #16</t>
+  </si>
+  <si>
+    <t>Fire #17</t>
+  </si>
+  <si>
+    <t>Fire #18</t>
+  </si>
+  <si>
+    <t>Fire #19</t>
+  </si>
+  <si>
+    <t>Fire #20</t>
+  </si>
+  <si>
+    <t>Fire #21</t>
+  </si>
+  <si>
+    <t>Fire #22</t>
+  </si>
+  <si>
+    <t>Fire #23</t>
+  </si>
+  <si>
+    <t>Fire #24</t>
+  </si>
+  <si>
+    <t>Fire #25</t>
+  </si>
+  <si>
+    <t>Fire #26</t>
+  </si>
+  <si>
+    <t>Fire #27</t>
+  </si>
+  <si>
+    <t>Fire #28</t>
+  </si>
+  <si>
+    <t>Fire #29</t>
+  </si>
+  <si>
+    <t>Fire #30</t>
+  </si>
+  <si>
+    <t>Fire #31</t>
+  </si>
+  <si>
+    <t>Fire #32</t>
+  </si>
+  <si>
+    <t>Fire #33</t>
+  </si>
+  <si>
+    <t>Fire #34</t>
+  </si>
+  <si>
+    <t>Fire #35</t>
+  </si>
+  <si>
+    <t>Fire #36</t>
+  </si>
+  <si>
+    <t>Fire #37</t>
+  </si>
+  <si>
+    <t>Fire #38</t>
+  </si>
+  <si>
+    <t>Fire #39</t>
+  </si>
+  <si>
+    <t>Fire #40</t>
+  </si>
+  <si>
+    <t>Fire #41</t>
+  </si>
+  <si>
+    <t>Fire #42</t>
+  </si>
+  <si>
+    <t>Fire #43</t>
+  </si>
+  <si>
+    <t>Fire #44</t>
+  </si>
+  <si>
+    <t>Fire #45</t>
+  </si>
+  <si>
+    <t>Fire #46</t>
+  </si>
+  <si>
+    <t>Fire #47</t>
+  </si>
+  <si>
+    <t>Fire #48</t>
+  </si>
+  <si>
+    <t>Fire #49</t>
+  </si>
+  <si>
+    <t>Fire #50</t>
   </si>
   <si>
     <t>timeElapsed</t>
@@ -1189,7 +1534,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1232,11 +1577,16 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1273,6 +1623,11 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1343,166 +1698,166 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>270</v>
+        <v>385</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>271</v>
+        <v>386</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>272</v>
+        <v>387</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>273</v>
+        <v>388</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>274</v>
+        <v>389</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>275</v>
+        <v>390</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>276</v>
+        <v>391</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>277</v>
+        <v>392</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>278</v>
+        <v>393</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>279</v>
+        <v>394</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>280</v>
+        <v>395</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>281</v>
+        <v>396</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>282</v>
+        <v>397</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>283</v>
+        <v>398</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>284</v>
+        <v>399</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>285</v>
+        <v>400</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>286</v>
+        <v>401</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>287</v>
+        <v>402</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>288</v>
+        <v>403</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>289</v>
+        <v>404</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>291</v>
+        <v>406</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>292</v>
+        <v>407</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>293</v>
+        <v>408</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>294</v>
+        <v>409</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>295</v>
+        <v>410</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>296</v>
+        <v>411</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>297</v>
+        <v>412</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>298</v>
+        <v>413</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>299</v>
+        <v>414</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>300</v>
+        <v>415</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>301</v>
+        <v>416</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>302</v>
+        <v>417</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>303</v>
+        <v>418</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>304</v>
+        <v>419</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>305</v>
+        <v>420</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>306</v>
+        <v>421</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>307</v>
+        <v>422</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>308</v>
+        <v>423</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>309</v>
+        <v>424</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>310</v>
+        <v>425</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>311</v>
+        <v>426</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>312</v>
+        <v>427</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>313</v>
+        <v>428</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>314</v>
+        <v>429</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>315</v>
+        <v>430</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>316</v>
+        <v>431</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>317</v>
+        <v>432</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>318</v>
+        <v>433</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>319</v>
+        <v>434</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>320</v>
+        <v>435</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>321</v>
+        <v>436</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>322</v>
+        <v>437</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>323</v>
+        <v>438</v>
       </c>
     </row>
     <row r="2">
@@ -1671,19 +2026,19 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>324</v>
+        <v>439</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>325</v>
+        <v>440</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>326</v>
+        <v>441</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>327</v>
+        <v>442</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>328</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5">
@@ -1705,19 +2060,19 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>329</v>
+        <v>444</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>330</v>
+        <v>445</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>331</v>
+        <v>446</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>332</v>
+        <v>447</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>333</v>
+        <v>448</v>
       </c>
     </row>
     <row r="8">
@@ -1739,154 +2094,154 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>334</v>
+        <v>449</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>335</v>
+        <v>450</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>336</v>
+        <v>451</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>337</v>
+        <v>452</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>338</v>
+        <v>453</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>339</v>
+        <v>454</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>340</v>
+        <v>455</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>341</v>
+        <v>456</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>342</v>
+        <v>457</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>343</v>
+        <v>458</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>344</v>
+        <v>459</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>345</v>
+        <v>460</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>346</v>
+        <v>461</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>347</v>
+        <v>462</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>348</v>
+        <v>463</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>349</v>
+        <v>464</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>350</v>
+        <v>465</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>351</v>
+        <v>466</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>352</v>
+        <v>467</v>
       </c>
       <c r="T10" s="0" t="s">
-        <v>353</v>
+        <v>468</v>
       </c>
       <c r="U10" s="0" t="s">
-        <v>354</v>
+        <v>469</v>
       </c>
       <c r="V10" s="0" t="s">
-        <v>355</v>
+        <v>470</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>356</v>
+        <v>471</v>
       </c>
       <c r="X10" s="0" t="s">
-        <v>357</v>
+        <v>472</v>
       </c>
       <c r="Y10" s="0" t="s">
-        <v>358</v>
+        <v>473</v>
       </c>
       <c r="Z10" s="0" t="s">
-        <v>359</v>
+        <v>474</v>
       </c>
       <c r="AA10" s="0" t="s">
-        <v>360</v>
+        <v>475</v>
       </c>
       <c r="AB10" s="0" t="s">
-        <v>361</v>
+        <v>476</v>
       </c>
       <c r="AC10" s="0" t="s">
-        <v>362</v>
+        <v>477</v>
       </c>
       <c r="AD10" s="0" t="s">
-        <v>363</v>
+        <v>478</v>
       </c>
       <c r="AE10" s="0" t="s">
-        <v>364</v>
+        <v>479</v>
       </c>
       <c r="AF10" s="0" t="s">
-        <v>365</v>
+        <v>480</v>
       </c>
       <c r="AG10" s="0" t="s">
-        <v>366</v>
+        <v>481</v>
       </c>
       <c r="AH10" s="0" t="s">
-        <v>367</v>
+        <v>482</v>
       </c>
       <c r="AI10" s="0" t="s">
-        <v>368</v>
+        <v>483</v>
       </c>
       <c r="AJ10" s="0" t="s">
-        <v>369</v>
+        <v>484</v>
       </c>
       <c r="AK10" s="0" t="s">
-        <v>370</v>
+        <v>485</v>
       </c>
       <c r="AL10" s="0" t="s">
-        <v>371</v>
+        <v>486</v>
       </c>
       <c r="AM10" s="0" t="s">
-        <v>372</v>
+        <v>487</v>
       </c>
       <c r="AN10" s="0" t="s">
-        <v>373</v>
+        <v>488</v>
       </c>
       <c r="AO10" s="0" t="s">
-        <v>374</v>
+        <v>489</v>
       </c>
       <c r="AP10" s="0" t="s">
-        <v>375</v>
+        <v>490</v>
       </c>
       <c r="AQ10" s="0" t="s">
-        <v>376</v>
+        <v>491</v>
       </c>
       <c r="AR10" s="0" t="s">
-        <v>377</v>
+        <v>492</v>
       </c>
       <c r="AS10" s="0" t="s">
-        <v>378</v>
+        <v>493</v>
       </c>
       <c r="AT10" s="0" t="s">
-        <v>379</v>
+        <v>494</v>
       </c>
       <c r="AU10" s="0" t="s">
-        <v>380</v>
+        <v>495</v>
       </c>
       <c r="AV10" s="0" t="s">
-        <v>381</v>
+        <v>496</v>
       </c>
       <c r="AW10" s="0" t="s">
-        <v>382</v>
+        <v>497</v>
       </c>
       <c r="AX10" s="0" t="s">
-        <v>383</v>
+        <v>498</v>
       </c>
     </row>
     <row r="11">
@@ -2043,12 +2398,12 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>384</v>
+        <v>499</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>104.1449846</v>
+        <v>104.3270289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>